<commit_message>
Improvement of Wdeel and BBX
</commit_message>
<xml_diff>
--- a/src/sastadev/data/methods/TARSP_Index_Current.xlsx
+++ b/src/sastadev/data/methods/TARSP_Index_Current.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\jodijk\myprograms\python\sastacode\mysastadev\src\sastadev\data\methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1097ED3D-B6FA-4B19-B294-55EC241B6887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439F61E0-3BE7-4E1E-9D91-1B41993C6B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,6 +19,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$V$156</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1663,9 +1664,6 @@
     <t>//node[%wxyz5%]</t>
   </si>
   <si>
-    <t>//node[%Tarsp_BBX%]</t>
-  </si>
-  <si>
     <t>//node[%Tarsp_Ov3%]</t>
   </si>
   <si>
@@ -1890,9 +1888,6 @@
     <t>tarsp_mvzn</t>
   </si>
   <si>
-    <t>//node[not(%bvbvraagwoord%) and (@pt='adj' or @pt='bw' or @pt='vz' or %Rpronounx%) and not(parent::node[@cat="sv1"]) and @lemma!="kijk" and ancestor::node[@cat="top" and  count(.//node[%realwordnode%])=1]]</t>
-  </si>
-  <si>
     <t>tarsp2005,tarsp2017</t>
   </si>
   <si>
@@ -1921,6 +1916,12 @@
   </si>
   <si>
     <t>//node[node[(@lemma="een" or @lemma="'n") and @pt="lid"] and node[(@pt="n" or (@pt="adj" and @positie="nom")) and @rel="hd"] and count(node)=2 ]</t>
+  </si>
+  <si>
+    <t>bbx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//node[%bvb% ] </t>
   </si>
 </sst>
 </file>
@@ -2341,11 +2342,11 @@
   <dimension ref="A1:V156"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="G21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="G14" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
-      <selection pane="bottomRight" activeCell="K30" sqref="K30"/>
+      <selection pane="bottomRight" activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2409,22 +2410,22 @@
         <v>443</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>554</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>555</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>556</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>557</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>558</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>158</v>
@@ -2444,13 +2445,13 @@
         <v>193</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>70</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>354</v>
@@ -2462,7 +2463,7 @@
         <v>3</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>354</v>
@@ -2556,7 +2557,7 @@
         <v>444</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
@@ -2620,7 +2621,7 @@
         <v>1</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>354</v>
@@ -2649,7 +2650,7 @@
         <v>193</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>354</v>
@@ -2775,7 +2776,7 @@
         <v>4</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>354</v>
@@ -2839,7 +2840,7 @@
         <v>38</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>354</v>
@@ -2851,7 +2852,7 @@
         <v>3</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>527</v>
+        <v>607</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>354</v>
@@ -3073,7 +3074,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>231</v>
       </c>
@@ -3087,7 +3088,7 @@
         <v>391</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>354</v>
@@ -3099,7 +3100,7 @@
         <v>1</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>599</v>
+        <v>608</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>354</v>
@@ -3166,7 +3167,7 @@
         <v>4</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="L21" s="2" t="s">
         <v>354</v>
@@ -3230,7 +3231,7 @@
         <v>47</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>354</v>
@@ -3274,7 +3275,7 @@
         <v>26</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>354</v>
@@ -3286,7 +3287,7 @@
         <v>2</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>354</v>
@@ -3464,7 +3465,7 @@
         <v>2</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="L29" s="2" t="s">
         <v>354</v>
@@ -3502,7 +3503,7 @@
         <v>3</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="L30" s="2" t="s">
         <v>354</v>
@@ -3552,7 +3553,7 @@
         <v>444</v>
       </c>
       <c r="R31" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
@@ -3622,7 +3623,7 @@
         <v>3</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="L33" s="2" t="s">
         <v>354</v>
@@ -3634,7 +3635,7 @@
         <v>444</v>
       </c>
       <c r="R33" s="2" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.3">
@@ -3660,7 +3661,7 @@
         <v>6</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="L34" s="2" t="s">
         <v>354</v>
@@ -3765,7 +3766,7 @@
         <v>3</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="L37" s="2" t="s">
         <v>354</v>
@@ -3794,7 +3795,7 @@
         <v>210</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>354</v>
@@ -3806,7 +3807,7 @@
         <v>364</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="L38" s="3" t="s">
         <v>354</v>
@@ -3835,7 +3836,7 @@
         <v>211</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>354</v>
@@ -3847,7 +3848,7 @@
         <v>4</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="L39" s="3" t="s">
         <v>354</v>
@@ -3873,7 +3874,7 @@
         <v>145</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>354</v>
@@ -4005,7 +4006,7 @@
         <v>3</v>
       </c>
       <c r="K43" s="3" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="L43" s="2" t="s">
         <v>354</v>
@@ -4110,7 +4111,7 @@
         <v>203</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="H46" s="2" t="s">
         <v>354</v>
@@ -4186,7 +4187,7 @@
         <v>355</v>
       </c>
       <c r="K48" s="3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="L48" s="3" t="s">
         <v>355</v>
@@ -4294,7 +4295,7 @@
         <v>4</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="L51" s="2" t="s">
         <v>354</v>
@@ -4332,7 +4333,7 @@
         <v>2</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="L52" s="2" t="s">
         <v>354</v>
@@ -4484,7 +4485,7 @@
         <v>444</v>
       </c>
       <c r="R56" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.3">
@@ -4510,7 +4511,7 @@
         <v>1</v>
       </c>
       <c r="K57" s="3" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="L57" s="2" t="s">
         <v>355</v>
@@ -4539,7 +4540,7 @@
         <v>21</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="H58" s="2" t="s">
         <v>354</v>
@@ -4551,7 +4552,7 @@
         <v>2</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="L58" s="2" t="s">
         <v>354</v>
@@ -4580,7 +4581,7 @@
         <v>39</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="H59" s="2" t="s">
         <v>354</v>
@@ -4592,7 +4593,7 @@
         <v>3</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L59" s="2" t="s">
         <v>354</v>
@@ -4642,7 +4643,7 @@
         <v>444</v>
       </c>
       <c r="R60" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.3">
@@ -4823,7 +4824,7 @@
         <v>2</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="L65" s="2" t="s">
         <v>354</v>
@@ -4852,7 +4853,7 @@
         <v>25</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="H66" s="2" t="s">
         <v>354</v>
@@ -4864,7 +4865,7 @@
         <v>2</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="L66" s="2" t="s">
         <v>354</v>
@@ -4893,7 +4894,7 @@
         <v>35</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="H67" s="2" t="s">
         <v>354</v>
@@ -4905,7 +4906,7 @@
         <v>3</v>
       </c>
       <c r="K67" s="3" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="L67" s="2" t="s">
         <v>354</v>
@@ -4934,7 +4935,7 @@
         <v>44</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="H68" s="2" t="s">
         <v>354</v>
@@ -4975,7 +4976,7 @@
         <v>43</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="H69" s="2" t="s">
         <v>354</v>
@@ -5016,7 +5017,7 @@
         <v>32</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H70" s="2" t="s">
         <v>354</v>
@@ -5057,7 +5058,7 @@
         <v>46</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H71" s="2" t="s">
         <v>354</v>
@@ -5098,10 +5099,10 @@
         <v>407</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="H72" s="2" t="s">
         <v>354</v>
@@ -5139,10 +5140,10 @@
         <v>188</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="H73" s="2" t="s">
         <v>354</v>
@@ -5154,7 +5155,7 @@
         <v>3</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="L73" s="2" t="s">
         <v>354</v>
@@ -5204,7 +5205,7 @@
         <v>444</v>
       </c>
       <c r="R74" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.3">
@@ -5239,7 +5240,7 @@
         <v>444</v>
       </c>
       <c r="R75" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.3">
@@ -5297,10 +5298,10 @@
         <v>49</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="H77" s="2" t="s">
         <v>354</v>
@@ -5341,10 +5342,10 @@
         <v>48</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="H78" s="2" t="s">
         <v>354</v>
@@ -5382,7 +5383,7 @@
         <v>139</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="H79" s="2" t="s">
         <v>354</v>
@@ -5406,7 +5407,7 @@
         <v>444</v>
       </c>
       <c r="R79" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="80" spans="1:21" x14ac:dyDescent="0.3">
@@ -5470,7 +5471,7 @@
         <v>4</v>
       </c>
       <c r="K81" s="3" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="L81" s="3" t="s">
         <v>354</v>
@@ -5508,7 +5509,7 @@
         <v>4</v>
       </c>
       <c r="K82" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="L82" s="2" t="s">
         <v>354</v>
@@ -5584,7 +5585,7 @@
         <v>444</v>
       </c>
       <c r="R84" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="85" spans="1:21" x14ac:dyDescent="0.3">
@@ -5709,7 +5710,7 @@
         <v>1</v>
       </c>
       <c r="K88" s="3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="L88" s="2" t="s">
         <v>354</v>
@@ -5884,7 +5885,7 @@
         <v>6</v>
       </c>
       <c r="K93" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="L93" s="2" t="s">
         <v>354</v>
@@ -5913,10 +5914,10 @@
         <v>24</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="H94" s="2" t="s">
         <v>354</v>
@@ -5928,7 +5929,7 @@
         <v>2</v>
       </c>
       <c r="K94" s="2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="L94" s="2" t="s">
         <v>354</v>
@@ -5960,7 +5961,7 @@
         <v>45</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="H95" s="2" t="s">
         <v>354</v>
@@ -6083,7 +6084,7 @@
         <v>444</v>
       </c>
       <c r="R98" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="99" spans="1:21" x14ac:dyDescent="0.3">
@@ -6112,7 +6113,7 @@
         <v>2</v>
       </c>
       <c r="K99" s="2" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L99" s="2" t="s">
         <v>354</v>
@@ -6188,7 +6189,7 @@
         <v>5</v>
       </c>
       <c r="K101" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="L101" s="2" t="s">
         <v>354</v>
@@ -6223,7 +6224,7 @@
         <v>4</v>
       </c>
       <c r="K102" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="L102" s="2" t="s">
         <v>354</v>
@@ -6311,7 +6312,7 @@
         <v>456</v>
       </c>
       <c r="R104" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="U104" s="2" t="s">
         <v>167</v>
@@ -6498,7 +6499,7 @@
         <v>6</v>
       </c>
       <c r="K109" s="3" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="L109" s="2" t="s">
         <v>354</v>
@@ -6543,7 +6544,7 @@
         <v>444</v>
       </c>
       <c r="R110" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="111" spans="1:21" x14ac:dyDescent="0.3">
@@ -6569,7 +6570,7 @@
         <v>4</v>
       </c>
       <c r="K111" s="2" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="L111" s="2" t="s">
         <v>354</v>
@@ -6605,7 +6606,7 @@
         <v>3</v>
       </c>
       <c r="K112" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="L112" s="2" t="s">
         <v>354</v>
@@ -6666,7 +6667,7 @@
         <v>193</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="H114" s="2" t="s">
         <v>354</v>
@@ -6678,7 +6679,7 @@
         <v>1</v>
       </c>
       <c r="K114" s="3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L114" s="2" t="s">
         <v>355</v>
@@ -6713,7 +6714,7 @@
         <v>1</v>
       </c>
       <c r="K115" s="3" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="L115" s="3" t="s">
         <v>354</v>
@@ -6745,7 +6746,7 @@
         <v>79</v>
       </c>
       <c r="G116" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="H116" s="2" t="s">
         <v>354</v>
@@ -6877,7 +6878,7 @@
         <v>40</v>
       </c>
       <c r="G120" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="H120" s="2" t="s">
         <v>354</v>
@@ -6924,7 +6925,7 @@
         <v>4</v>
       </c>
       <c r="K121" s="2" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="L121" s="2" t="s">
         <v>354</v>
@@ -7023,10 +7024,10 @@
         <v>71</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="G124" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="H124" s="2" t="s">
         <v>354</v>
@@ -7067,7 +7068,7 @@
         <v>73</v>
       </c>
       <c r="G125" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="H125" s="2" t="s">
         <v>354</v>
@@ -7111,7 +7112,7 @@
         <v>75</v>
       </c>
       <c r="G126" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="H126" s="2" t="s">
         <v>354</v>
@@ -7254,7 +7255,7 @@
         <v>80</v>
       </c>
       <c r="G130" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="H130" s="2" t="s">
         <v>354</v>
@@ -7295,7 +7296,7 @@
         <v>81</v>
       </c>
       <c r="G131" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="H131" s="2" t="s">
         <v>354</v>
@@ -7339,7 +7340,7 @@
         <v>442</v>
       </c>
       <c r="G132" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="H132" s="2" t="s">
         <v>354</v>
@@ -7464,7 +7465,7 @@
         <v>205</v>
       </c>
       <c r="G135" s="10" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="H135" s="2" t="s">
         <v>354</v>
@@ -7476,7 +7477,7 @@
         <v>3</v>
       </c>
       <c r="K135" s="3" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="L135" s="2" t="s">
         <v>354</v>
@@ -7628,7 +7629,7 @@
         <v>444</v>
       </c>
       <c r="R139" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="140" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
@@ -7645,7 +7646,7 @@
         <v>6</v>
       </c>
       <c r="F140" s="2" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="H140" s="2" t="s">
         <v>354</v>
@@ -7657,7 +7658,7 @@
         <v>1</v>
       </c>
       <c r="K140" s="3" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="L140" s="2" t="s">
         <v>354</v>
@@ -7922,7 +7923,7 @@
         <v>411</v>
       </c>
       <c r="F148" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="H148" s="2" t="s">
         <v>354</v>
@@ -8103,7 +8104,7 @@
         <v>445</v>
       </c>
       <c r="R153" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="154" spans="1:21" x14ac:dyDescent="0.3">
@@ -8163,7 +8164,7 @@
     </row>
     <row r="156" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="B156" s="2" t="s">
         <v>125</v>
@@ -8175,34 +8176,34 @@
         <v>139</v>
       </c>
       <c r="F156" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="H156" s="2" t="s">
         <v>354</v>
       </c>
       <c r="I156" s="2" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="J156" s="2">
         <v>6</v>
       </c>
       <c r="K156" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="L156" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="M156" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="N156" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="R156" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="U156" s="2" t="s">
         <v>605</v>
-      </c>
-      <c r="L156" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="M156" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="N156" s="2" t="s">
-        <v>444</v>
-      </c>
-      <c r="R156" s="2" t="s">
-        <v>606</v>
-      </c>
-      <c r="U156" s="2" t="s">
-        <v>607</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
vuwords update, locverb update
</commit_message>
<xml_diff>
--- a/src/sastadev/data/methods/TARSP_Index_Current.xlsx
+++ b/src/sastadev/data/methods/TARSP_Index_Current.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\jodijk\myprograms\python\sastacode\mysastadev\src\sastadev\data\methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439F61E0-3BE7-4E1E-9D91-1B41993C6B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F94BEA5-655D-4B65-B11C-69377E7F1520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$V$156</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1185,9 +1184,6 @@
     <t>we must require a finite verb, but prbaly not too deep (incl. mensen die zwemmen should not do!)</t>
   </si>
   <si>
-    <t>//node[@rel="mod"and @cat="cp" and node[@rel="body" and node[@pt="ww" and @pvagr and @rel="hd"]]]</t>
-  </si>
-  <si>
     <t>//node[@rel="su" and @cat]</t>
   </si>
   <si>
@@ -1922,6 +1918,9 @@
   </si>
   <si>
     <t xml:space="preserve">//node[%bvb% ] </t>
+  </si>
+  <si>
+    <t>//node[@rel="mod"and @cat="cp" and not(%Tarsp_ofmod%) and  node[@rel="body" and node[@pt="ww" and @pvagr and @rel="hd"]]]</t>
   </si>
 </sst>
 </file>
@@ -2342,11 +2341,11 @@
   <dimension ref="A1:V156"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="G14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="G8" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
-      <selection pane="bottomRight" activeCell="K19" sqref="K19"/>
+      <selection pane="bottomRight" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2401,31 +2400,31 @@
         <v>157</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>553</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>554</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>555</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>556</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>557</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>158</v>
@@ -2445,13 +2444,13 @@
         <v>193</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>70</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>354</v>
@@ -2463,7 +2462,7 @@
         <v>3</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>354</v>
@@ -2472,10 +2471,10 @@
         <v>355</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
@@ -2504,7 +2503,7 @@
         <v>6</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>354</v>
@@ -2513,10 +2512,10 @@
         <v>354</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
@@ -2533,7 +2532,7 @@
         <v>193</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>63</v>
@@ -2554,10 +2553,10 @@
         <v>355</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
@@ -2592,7 +2591,7 @@
         <v>355</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="U5" s="2" t="s">
         <v>185</v>
@@ -2621,7 +2620,7 @@
         <v>1</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>354</v>
@@ -2630,13 +2629,13 @@
         <v>355</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="U6" s="2" t="s">
         <v>360</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
@@ -2650,7 +2649,7 @@
         <v>193</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>354</v>
@@ -2662,7 +2661,7 @@
         <v>1</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>355</v>
@@ -2671,7 +2670,7 @@
         <v>355</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
@@ -2709,7 +2708,7 @@
         <v>355</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.3">
@@ -2738,7 +2737,7 @@
         <v>6</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>375</v>
+        <v>608</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>354</v>
@@ -2747,7 +2746,7 @@
         <v>354</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="U9" s="2" t="s">
         <v>374</v>
@@ -2776,7 +2775,7 @@
         <v>4</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>354</v>
@@ -2785,7 +2784,7 @@
         <v>355</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
@@ -2820,7 +2819,7 @@
         <v>355</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.3">
@@ -2840,7 +2839,7 @@
         <v>38</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>354</v>
@@ -2852,7 +2851,7 @@
         <v>3</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>354</v>
@@ -2861,7 +2860,7 @@
         <v>355</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
@@ -2896,7 +2895,7 @@
         <v>355</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.3">
@@ -2925,7 +2924,7 @@
         <v>4</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>355</v>
@@ -2934,7 +2933,7 @@
         <v>355</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="15" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
@@ -2960,7 +2959,7 @@
         <v>4</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>354</v>
@@ -2969,7 +2968,7 @@
         <v>355</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.3">
@@ -2989,7 +2988,7 @@
         <v>354</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>355</v>
@@ -2998,7 +2997,7 @@
         <v>355</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.3">
@@ -3030,7 +3029,7 @@
         <v>354</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.3">
@@ -3047,10 +3046,10 @@
         <v>193</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>354</v>
@@ -3068,10 +3067,10 @@
         <v>355</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.3">
@@ -3085,10 +3084,10 @@
         <v>193</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>354</v>
@@ -3100,7 +3099,7 @@
         <v>1</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>354</v>
@@ -3109,7 +3108,7 @@
         <v>354</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.3">
@@ -3141,7 +3140,7 @@
         <v>355</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.3">
@@ -3167,7 +3166,7 @@
         <v>4</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="L21" s="2" t="s">
         <v>354</v>
@@ -3176,7 +3175,7 @@
         <v>355</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.3">
@@ -3202,7 +3201,7 @@
         <v>3</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="L22" s="2" t="s">
         <v>354</v>
@@ -3211,7 +3210,7 @@
         <v>355</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.3">
@@ -3231,7 +3230,7 @@
         <v>47</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>354</v>
@@ -3243,7 +3242,7 @@
         <v>5</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L23" s="2" t="s">
         <v>354</v>
@@ -3252,7 +3251,7 @@
         <v>355</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3269,13 +3268,13 @@
         <v>193</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>354</v>
@@ -3287,7 +3286,7 @@
         <v>2</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>354</v>
@@ -3296,10 +3295,10 @@
         <v>355</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="U24" s="3" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.3">
@@ -3331,7 +3330,7 @@
         <v>355</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
@@ -3357,7 +3356,7 @@
         <v>4</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="L26" s="3" t="s">
         <v>354</v>
@@ -3366,10 +3365,10 @@
         <v>355</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="U26" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.3">
@@ -3404,7 +3403,7 @@
         <v>355</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.3">
@@ -3439,7 +3438,7 @@
         <v>354</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.3">
@@ -3465,7 +3464,7 @@
         <v>2</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="L29" s="2" t="s">
         <v>354</v>
@@ -3474,7 +3473,7 @@
         <v>355</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="U29" s="2" t="s">
         <v>372</v>
@@ -3503,7 +3502,7 @@
         <v>3</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="L30" s="2" t="s">
         <v>354</v>
@@ -3512,7 +3511,7 @@
         <v>354</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="U30" s="2" t="s">
         <v>185</v>
@@ -3550,10 +3549,10 @@
         <v>355</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="R31" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
@@ -3591,7 +3590,7 @@
         <v>355</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.3">
@@ -3623,7 +3622,7 @@
         <v>3</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="L33" s="2" t="s">
         <v>354</v>
@@ -3632,10 +3631,10 @@
         <v>355</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="R33" s="2" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.3">
@@ -3661,7 +3660,7 @@
         <v>6</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="L34" s="2" t="s">
         <v>354</v>
@@ -3670,7 +3669,7 @@
         <v>355</v>
       </c>
       <c r="N34" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.3">
@@ -3705,7 +3704,7 @@
         <v>354</v>
       </c>
       <c r="N35" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="36" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
@@ -3740,7 +3739,7 @@
         <v>354</v>
       </c>
       <c r="N36" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.3">
@@ -3766,7 +3765,7 @@
         <v>3</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="L37" s="2" t="s">
         <v>354</v>
@@ -3775,7 +3774,7 @@
         <v>355</v>
       </c>
       <c r="N37" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.3">
@@ -3795,7 +3794,7 @@
         <v>210</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>354</v>
@@ -3807,7 +3806,7 @@
         <v>364</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="L38" s="3" t="s">
         <v>354</v>
@@ -3816,7 +3815,7 @@
         <v>355</v>
       </c>
       <c r="N38" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.3">
@@ -3836,7 +3835,7 @@
         <v>211</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>354</v>
@@ -3848,7 +3847,7 @@
         <v>4</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="L39" s="3" t="s">
         <v>354</v>
@@ -3857,7 +3856,7 @@
         <v>355</v>
       </c>
       <c r="N39" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.3">
@@ -3874,7 +3873,7 @@
         <v>145</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>354</v>
@@ -3886,7 +3885,7 @@
         <v>3</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="L40" s="3" t="s">
         <v>354</v>
@@ -3895,10 +3894,10 @@
         <v>354</v>
       </c>
       <c r="N40" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="U40" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.3">
@@ -3933,7 +3932,7 @@
         <v>354</v>
       </c>
       <c r="N41" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.3">
@@ -3953,7 +3952,7 @@
         <v>67</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>354</v>
@@ -3971,7 +3970,7 @@
         <v>355</v>
       </c>
       <c r="N42" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="U42" s="2" t="s">
         <v>161</v>
@@ -3991,10 +3990,10 @@
         <v>193</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>354</v>
@@ -4006,7 +4005,7 @@
         <v>3</v>
       </c>
       <c r="K43" s="3" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="L43" s="2" t="s">
         <v>354</v>
@@ -4015,7 +4014,7 @@
         <v>355</v>
       </c>
       <c r="N43" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="U43" s="2" t="s">
         <v>359</v>
@@ -4044,7 +4043,7 @@
         <v>3</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="L44" s="2" t="s">
         <v>354</v>
@@ -4053,7 +4052,7 @@
         <v>355</v>
       </c>
       <c r="N44" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="45" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
@@ -4079,7 +4078,7 @@
         <v>6</v>
       </c>
       <c r="K45" s="3" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="L45" s="2" t="s">
         <v>354</v>
@@ -4088,7 +4087,7 @@
         <v>355</v>
       </c>
       <c r="N45" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.3">
@@ -4111,7 +4110,7 @@
         <v>203</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="H46" s="2" t="s">
         <v>354</v>
@@ -4123,7 +4122,7 @@
         <v>2</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="L46" s="2" t="s">
         <v>354</v>
@@ -4132,7 +4131,7 @@
         <v>355</v>
       </c>
       <c r="N46" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="47" spans="1:21" ht="86.4" x14ac:dyDescent="0.3">
@@ -4158,7 +4157,7 @@
         <v>6</v>
       </c>
       <c r="K47" s="3" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="L47" s="2" t="s">
         <v>354</v>
@@ -4167,7 +4166,7 @@
         <v>355</v>
       </c>
       <c r="N47" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="U47" s="2" t="s">
         <v>185</v>
@@ -4187,7 +4186,7 @@
         <v>355</v>
       </c>
       <c r="K48" s="3" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="L48" s="3" t="s">
         <v>355</v>
@@ -4196,7 +4195,7 @@
         <v>355</v>
       </c>
       <c r="N48" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="U48" s="6" t="s">
         <v>180</v>
@@ -4234,7 +4233,7 @@
         <v>355</v>
       </c>
       <c r="N49" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="50" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
@@ -4260,7 +4259,7 @@
         <v>5</v>
       </c>
       <c r="K50" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="L50" s="2" t="s">
         <v>354</v>
@@ -4269,7 +4268,7 @@
         <v>355</v>
       </c>
       <c r="N50" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.3">
@@ -4295,7 +4294,7 @@
         <v>4</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L51" s="2" t="s">
         <v>354</v>
@@ -4304,7 +4303,7 @@
         <v>355</v>
       </c>
       <c r="N51" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.3">
@@ -4333,7 +4332,7 @@
         <v>2</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L52" s="2" t="s">
         <v>354</v>
@@ -4342,7 +4341,7 @@
         <v>355</v>
       </c>
       <c r="N52" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.3">
@@ -4368,7 +4367,7 @@
         <v>6</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="L53" s="2" t="s">
         <v>354</v>
@@ -4377,7 +4376,7 @@
         <v>355</v>
       </c>
       <c r="N53" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.3">
@@ -4406,7 +4405,7 @@
         <v>6</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="L54" s="2" t="s">
         <v>354</v>
@@ -4415,7 +4414,7 @@
         <v>355</v>
       </c>
       <c r="N54" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.3">
@@ -4450,7 +4449,7 @@
         <v>354</v>
       </c>
       <c r="N55" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.3">
@@ -4482,10 +4481,10 @@
         <v>355</v>
       </c>
       <c r="N56" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="R56" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.3">
@@ -4511,7 +4510,7 @@
         <v>1</v>
       </c>
       <c r="K57" s="3" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="L57" s="2" t="s">
         <v>355</v>
@@ -4520,7 +4519,7 @@
         <v>355</v>
       </c>
       <c r="N57" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.3">
@@ -4540,7 +4539,7 @@
         <v>21</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="H58" s="2" t="s">
         <v>354</v>
@@ -4552,7 +4551,7 @@
         <v>2</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="L58" s="2" t="s">
         <v>354</v>
@@ -4561,7 +4560,7 @@
         <v>354</v>
       </c>
       <c r="N58" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.3">
@@ -4581,7 +4580,7 @@
         <v>39</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="H59" s="2" t="s">
         <v>354</v>
@@ -4593,7 +4592,7 @@
         <v>3</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="L59" s="2" t="s">
         <v>354</v>
@@ -4602,7 +4601,7 @@
         <v>355</v>
       </c>
       <c r="N59" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.3">
@@ -4619,7 +4618,7 @@
         <v>193</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>65</v>
@@ -4640,10 +4639,10 @@
         <v>355</v>
       </c>
       <c r="N60" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="R60" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.3">
@@ -4678,10 +4677,10 @@
         <v>355</v>
       </c>
       <c r="N61" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="U61" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.3">
@@ -4716,10 +4715,10 @@
         <v>355</v>
       </c>
       <c r="N62" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="U62" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.3">
@@ -4754,10 +4753,10 @@
         <v>355</v>
       </c>
       <c r="N63" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="U63" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="64" spans="1:21" x14ac:dyDescent="0.3">
@@ -4783,7 +4782,7 @@
         <v>4</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="L64" s="2" t="s">
         <v>355</v>
@@ -4792,7 +4791,7 @@
         <v>354</v>
       </c>
       <c r="N64" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.3">
@@ -4824,7 +4823,7 @@
         <v>2</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="L65" s="2" t="s">
         <v>354</v>
@@ -4833,7 +4832,7 @@
         <v>354</v>
       </c>
       <c r="N65" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="66" spans="1:21" x14ac:dyDescent="0.3">
@@ -4853,7 +4852,7 @@
         <v>25</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="H66" s="2" t="s">
         <v>354</v>
@@ -4865,7 +4864,7 @@
         <v>2</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="L66" s="2" t="s">
         <v>354</v>
@@ -4874,7 +4873,7 @@
         <v>354</v>
       </c>
       <c r="N66" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.3">
@@ -4894,7 +4893,7 @@
         <v>35</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="H67" s="2" t="s">
         <v>354</v>
@@ -4906,7 +4905,7 @@
         <v>3</v>
       </c>
       <c r="K67" s="3" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L67" s="2" t="s">
         <v>354</v>
@@ -4915,7 +4914,7 @@
         <v>355</v>
       </c>
       <c r="N67" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.3">
@@ -4935,7 +4934,7 @@
         <v>44</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="H68" s="2" t="s">
         <v>354</v>
@@ -4947,7 +4946,7 @@
         <v>4</v>
       </c>
       <c r="K68" s="3" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="L68" s="2" t="s">
         <v>354</v>
@@ -4956,7 +4955,7 @@
         <v>355</v>
       </c>
       <c r="N68" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.3">
@@ -4976,7 +4975,7 @@
         <v>43</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="H69" s="2" t="s">
         <v>354</v>
@@ -4988,7 +4987,7 @@
         <v>4</v>
       </c>
       <c r="K69" s="3" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="L69" s="2" t="s">
         <v>354</v>
@@ -4997,7 +4996,7 @@
         <v>354</v>
       </c>
       <c r="N69" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.3">
@@ -5017,7 +5016,7 @@
         <v>32</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="H70" s="2" t="s">
         <v>354</v>
@@ -5029,7 +5028,7 @@
         <v>3</v>
       </c>
       <c r="K70" s="3" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="L70" s="2" t="s">
         <v>354</v>
@@ -5038,7 +5037,7 @@
         <v>354</v>
       </c>
       <c r="N70" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.3">
@@ -5058,7 +5057,7 @@
         <v>46</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H71" s="2" t="s">
         <v>354</v>
@@ -5070,7 +5069,7 @@
         <v>5</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="L71" s="2" t="s">
         <v>354</v>
@@ -5079,7 +5078,7 @@
         <v>354</v>
       </c>
       <c r="N71" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.3">
@@ -5096,13 +5095,13 @@
         <v>193</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="H72" s="2" t="s">
         <v>354</v>
@@ -5120,7 +5119,7 @@
         <v>355</v>
       </c>
       <c r="N72" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="73" spans="1:21" x14ac:dyDescent="0.3">
@@ -5140,10 +5139,10 @@
         <v>188</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="H73" s="2" t="s">
         <v>354</v>
@@ -5155,7 +5154,7 @@
         <v>3</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="L73" s="2" t="s">
         <v>354</v>
@@ -5164,7 +5163,7 @@
         <v>355</v>
       </c>
       <c r="N73" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="74" spans="1:21" x14ac:dyDescent="0.3">
@@ -5184,7 +5183,7 @@
         <v>189</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H74" s="2" t="s">
         <v>354</v>
@@ -5202,10 +5201,10 @@
         <v>355</v>
       </c>
       <c r="N74" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="R74" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.3">
@@ -5237,10 +5236,10 @@
         <v>355</v>
       </c>
       <c r="N75" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="R75" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.3">
@@ -5257,7 +5256,7 @@
         <v>191</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H76" s="2" t="s">
         <v>354</v>
@@ -5275,7 +5274,7 @@
         <v>355</v>
       </c>
       <c r="N76" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="U76" s="2" t="s">
         <v>186</v>
@@ -5298,10 +5297,10 @@
         <v>49</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="H77" s="2" t="s">
         <v>354</v>
@@ -5313,7 +5312,7 @@
         <v>4</v>
       </c>
       <c r="K77" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="L77" s="2" t="s">
         <v>354</v>
@@ -5322,7 +5321,7 @@
         <v>355</v>
       </c>
       <c r="N77" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.3">
@@ -5342,10 +5341,10 @@
         <v>48</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="H78" s="2" t="s">
         <v>354</v>
@@ -5357,7 +5356,7 @@
         <v>5</v>
       </c>
       <c r="K78" s="3" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="L78" s="2" t="s">
         <v>354</v>
@@ -5366,7 +5365,7 @@
         <v>355</v>
       </c>
       <c r="N78" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="79" spans="1:21" x14ac:dyDescent="0.3">
@@ -5383,7 +5382,7 @@
         <v>139</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="H79" s="2" t="s">
         <v>354</v>
@@ -5395,7 +5394,7 @@
         <v>6</v>
       </c>
       <c r="K79" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="L79" s="2" t="s">
         <v>354</v>
@@ -5404,10 +5403,10 @@
         <v>355</v>
       </c>
       <c r="N79" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="R79" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="80" spans="1:21" x14ac:dyDescent="0.3">
@@ -5442,7 +5441,7 @@
         <v>355</v>
       </c>
       <c r="N80" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="U80" s="2" t="s">
         <v>164</v>
@@ -5471,7 +5470,7 @@
         <v>4</v>
       </c>
       <c r="K81" s="3" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="L81" s="3" t="s">
         <v>354</v>
@@ -5480,7 +5479,7 @@
         <v>355</v>
       </c>
       <c r="N81" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="82" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
@@ -5497,7 +5496,7 @@
         <v>150</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="H82" s="2" t="s">
         <v>354</v>
@@ -5509,7 +5508,7 @@
         <v>4</v>
       </c>
       <c r="K82" s="3" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="L82" s="2" t="s">
         <v>354</v>
@@ -5518,7 +5517,7 @@
         <v>355</v>
       </c>
       <c r="N82" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="83" spans="1:21" ht="115.2" x14ac:dyDescent="0.3">
@@ -5544,7 +5543,7 @@
         <v>355</v>
       </c>
       <c r="N83" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="84" spans="1:21" ht="115.2" x14ac:dyDescent="0.3">
@@ -5582,10 +5581,10 @@
         <v>355</v>
       </c>
       <c r="N84" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="R84" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="85" spans="1:21" x14ac:dyDescent="0.3">
@@ -5617,7 +5616,7 @@
         <v>355</v>
       </c>
       <c r="N85" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="86" spans="1:21" x14ac:dyDescent="0.3">
@@ -5649,7 +5648,7 @@
         <v>355</v>
       </c>
       <c r="N86" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.3">
@@ -5681,7 +5680,7 @@
         <v>355</v>
       </c>
       <c r="N87" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="88" spans="1:21" x14ac:dyDescent="0.3">
@@ -5695,10 +5694,10 @@
         <v>193</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="H88" s="2" t="s">
         <v>354</v>
@@ -5710,7 +5709,7 @@
         <v>1</v>
       </c>
       <c r="K88" s="3" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="L88" s="2" t="s">
         <v>354</v>
@@ -5719,7 +5718,7 @@
         <v>355</v>
       </c>
       <c r="N88" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.3">
@@ -5733,7 +5732,7 @@
         <v>193</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="H89" s="2" t="s">
         <v>354</v>
@@ -5745,7 +5744,7 @@
         <v>1</v>
       </c>
       <c r="K89" s="2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="L89" s="2" t="s">
         <v>354</v>
@@ -5754,7 +5753,7 @@
         <v>355</v>
       </c>
       <c r="N89" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.3">
@@ -5768,10 +5767,10 @@
         <v>193</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="H90" s="2" t="s">
         <v>354</v>
@@ -5789,12 +5788,12 @@
         <v>355</v>
       </c>
       <c r="N90" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="91" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>2</v>
@@ -5803,22 +5802,22 @@
         <v>193</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="H91" s="2" t="s">
         <v>354</v>
       </c>
       <c r="I91" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="J91" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="J91" s="2" t="s">
-        <v>387</v>
-      </c>
       <c r="K91" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L91" s="2" t="s">
         <v>354</v>
@@ -5827,7 +5826,7 @@
         <v>355</v>
       </c>
       <c r="N91" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.3">
@@ -5844,7 +5843,7 @@
         <v>354</v>
       </c>
       <c r="K92" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="L92" s="2" t="s">
         <v>355</v>
@@ -5853,7 +5852,7 @@
         <v>355</v>
       </c>
       <c r="N92" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.3">
@@ -5873,7 +5872,7 @@
         <v>59</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H93" s="2" t="s">
         <v>354</v>
@@ -5885,7 +5884,7 @@
         <v>6</v>
       </c>
       <c r="K93" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L93" s="2" t="s">
         <v>354</v>
@@ -5894,7 +5893,7 @@
         <v>354</v>
       </c>
       <c r="N93" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.3">
@@ -5914,10 +5913,10 @@
         <v>24</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H94" s="2" t="s">
         <v>354</v>
@@ -5929,7 +5928,7 @@
         <v>2</v>
       </c>
       <c r="K94" s="2" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="L94" s="2" t="s">
         <v>354</v>
@@ -5938,7 +5937,7 @@
         <v>354</v>
       </c>
       <c r="N94" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="U94" s="2" t="s">
         <v>159</v>
@@ -5961,7 +5960,7 @@
         <v>45</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="H95" s="2" t="s">
         <v>354</v>
@@ -5973,7 +5972,7 @@
         <v>5</v>
       </c>
       <c r="K95" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="L95" s="2" t="s">
         <v>354</v>
@@ -5982,7 +5981,7 @@
         <v>354</v>
       </c>
       <c r="N95" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="96" spans="1:21" x14ac:dyDescent="0.3">
@@ -6008,7 +6007,7 @@
         <v>3</v>
       </c>
       <c r="K96" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="L96" s="2" t="s">
         <v>355</v>
@@ -6017,7 +6016,7 @@
         <v>354</v>
       </c>
       <c r="N96" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="97" spans="1:21" ht="129.6" x14ac:dyDescent="0.3">
@@ -6034,13 +6033,13 @@
         <v>354</v>
       </c>
       <c r="I97" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="J97" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="K97" s="3" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="L97" s="3" t="s">
         <v>354</v>
@@ -6049,7 +6048,7 @@
         <v>355</v>
       </c>
       <c r="N97" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="98" spans="1:21" x14ac:dyDescent="0.3">
@@ -6081,10 +6080,10 @@
         <v>355</v>
       </c>
       <c r="N98" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="R98" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="99" spans="1:21" x14ac:dyDescent="0.3">
@@ -6098,7 +6097,7 @@
         <v>195</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F99" s="2" t="s">
         <v>142</v>
@@ -6113,7 +6112,7 @@
         <v>2</v>
       </c>
       <c r="K99" s="2" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="L99" s="2" t="s">
         <v>354</v>
@@ -6122,10 +6121,10 @@
         <v>355</v>
       </c>
       <c r="N99" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="P99" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="100" spans="1:21" x14ac:dyDescent="0.3">
@@ -6142,7 +6141,7 @@
         <v>153</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="H100" s="2" t="s">
         <v>354</v>
@@ -6154,7 +6153,7 @@
         <v>6</v>
       </c>
       <c r="K100" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="L100" s="2" t="s">
         <v>354</v>
@@ -6163,7 +6162,7 @@
         <v>354</v>
       </c>
       <c r="N100" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="101" spans="1:21" x14ac:dyDescent="0.3">
@@ -6189,7 +6188,7 @@
         <v>5</v>
       </c>
       <c r="K101" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="L101" s="2" t="s">
         <v>354</v>
@@ -6198,7 +6197,7 @@
         <v>355</v>
       </c>
       <c r="N101" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="102" spans="1:21" x14ac:dyDescent="0.3">
@@ -6224,7 +6223,7 @@
         <v>4</v>
       </c>
       <c r="K102" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="L102" s="2" t="s">
         <v>354</v>
@@ -6233,7 +6232,7 @@
         <v>355</v>
       </c>
       <c r="N102" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="103" spans="1:21" x14ac:dyDescent="0.3">
@@ -6271,7 +6270,7 @@
         <v>355</v>
       </c>
       <c r="N103" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="104" spans="1:21" x14ac:dyDescent="0.3">
@@ -6285,10 +6284,10 @@
         <v>195</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H104" s="2" t="s">
         <v>354</v>
@@ -6306,13 +6305,13 @@
         <v>355</v>
       </c>
       <c r="N104" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="P104" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="R104" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="U104" s="2" t="s">
         <v>167</v>
@@ -6341,7 +6340,7 @@
         <v>355</v>
       </c>
       <c r="N105" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="U105" s="2" t="s">
         <v>358</v>
@@ -6376,7 +6375,7 @@
         <v>4</v>
       </c>
       <c r="K106" s="3" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="L106" s="2" t="s">
         <v>354</v>
@@ -6385,7 +6384,7 @@
         <v>355</v>
       </c>
       <c r="N106" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="U106" s="2" t="s">
         <v>162</v>
@@ -6417,7 +6416,7 @@
         <v>5</v>
       </c>
       <c r="K107" s="3" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="L107" s="2" t="s">
         <v>354</v>
@@ -6426,10 +6425,10 @@
         <v>355</v>
       </c>
       <c r="N107" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="U107" s="2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="108" spans="1:21" x14ac:dyDescent="0.3">
@@ -6458,7 +6457,7 @@
         <v>6</v>
       </c>
       <c r="K108" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L108" s="2" t="s">
         <v>354</v>
@@ -6467,10 +6466,10 @@
         <v>354</v>
       </c>
       <c r="N108" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="P108" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="U108" s="2" t="s">
         <v>162</v>
@@ -6499,7 +6498,7 @@
         <v>6</v>
       </c>
       <c r="K109" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="L109" s="2" t="s">
         <v>354</v>
@@ -6508,7 +6507,7 @@
         <v>355</v>
       </c>
       <c r="N109" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="110" spans="1:21" x14ac:dyDescent="0.3">
@@ -6541,10 +6540,10 @@
         <v>355</v>
       </c>
       <c r="N110" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="R110" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="111" spans="1:21" x14ac:dyDescent="0.3">
@@ -6570,7 +6569,7 @@
         <v>4</v>
       </c>
       <c r="K111" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="L111" s="2" t="s">
         <v>354</v>
@@ -6579,7 +6578,7 @@
         <v>354</v>
       </c>
       <c r="N111" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="112" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -6606,7 +6605,7 @@
         <v>3</v>
       </c>
       <c r="K112" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="L112" s="2" t="s">
         <v>354</v>
@@ -6615,10 +6614,10 @@
         <v>355</v>
       </c>
       <c r="N112" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="U112" s="3" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="113" spans="1:21" x14ac:dyDescent="0.3">
@@ -6653,7 +6652,7 @@
         <v>355</v>
       </c>
       <c r="N113" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="114" spans="1:21" x14ac:dyDescent="0.3">
@@ -6667,7 +6666,7 @@
         <v>193</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="H114" s="2" t="s">
         <v>354</v>
@@ -6679,7 +6678,7 @@
         <v>1</v>
       </c>
       <c r="K114" s="3" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="L114" s="2" t="s">
         <v>355</v>
@@ -6688,7 +6687,7 @@
         <v>354</v>
       </c>
       <c r="N114" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="115" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
@@ -6714,7 +6713,7 @@
         <v>1</v>
       </c>
       <c r="K115" s="3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="L115" s="3" t="s">
         <v>354</v>
@@ -6723,10 +6722,10 @@
         <v>355</v>
       </c>
       <c r="N115" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="U115" s="2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="116" spans="1:21" x14ac:dyDescent="0.3">
@@ -6746,7 +6745,7 @@
         <v>79</v>
       </c>
       <c r="G116" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="H116" s="2" t="s">
         <v>354</v>
@@ -6758,7 +6757,7 @@
         <v>3</v>
       </c>
       <c r="K116" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="L116" s="2" t="s">
         <v>354</v>
@@ -6767,7 +6766,7 @@
         <v>355</v>
       </c>
       <c r="N116" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="117" spans="1:21" x14ac:dyDescent="0.3">
@@ -6795,7 +6794,7 @@
         <v>355</v>
       </c>
       <c r="N117" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="118" spans="1:21" x14ac:dyDescent="0.3">
@@ -6820,7 +6819,7 @@
         <v>355</v>
       </c>
       <c r="N118" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="119" spans="1:21" x14ac:dyDescent="0.3">
@@ -6855,7 +6854,7 @@
         <v>355</v>
       </c>
       <c r="N119" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="U119" s="2" t="s">
         <v>185</v>
@@ -6878,7 +6877,7 @@
         <v>40</v>
       </c>
       <c r="G120" s="2" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="H120" s="2" t="s">
         <v>354</v>
@@ -6890,7 +6889,7 @@
         <v>3</v>
       </c>
       <c r="K120" s="3" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="L120" s="2" t="s">
         <v>354</v>
@@ -6899,7 +6898,7 @@
         <v>355</v>
       </c>
       <c r="N120" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="121" spans="1:21" x14ac:dyDescent="0.3">
@@ -6925,7 +6924,7 @@
         <v>4</v>
       </c>
       <c r="K121" s="2" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="L121" s="2" t="s">
         <v>354</v>
@@ -6934,7 +6933,7 @@
         <v>355</v>
       </c>
       <c r="N121" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="122" spans="1:21" x14ac:dyDescent="0.3">
@@ -6960,7 +6959,7 @@
         <v>3</v>
       </c>
       <c r="K122" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="L122" s="2" t="s">
         <v>355</v>
@@ -6969,7 +6968,7 @@
         <v>354</v>
       </c>
       <c r="N122" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="123" spans="1:21" x14ac:dyDescent="0.3">
@@ -7004,7 +7003,7 @@
         <v>354</v>
       </c>
       <c r="N123" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="124" spans="1:21" x14ac:dyDescent="0.3">
@@ -7024,10 +7023,10 @@
         <v>71</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="G124" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="H124" s="2" t="s">
         <v>354</v>
@@ -7039,7 +7038,7 @@
         <v>4</v>
       </c>
       <c r="K124" s="3" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="L124" s="2" t="s">
         <v>354</v>
@@ -7048,7 +7047,7 @@
         <v>355</v>
       </c>
       <c r="N124" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="125" spans="1:21" x14ac:dyDescent="0.3">
@@ -7068,7 +7067,7 @@
         <v>73</v>
       </c>
       <c r="G125" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="H125" s="2" t="s">
         <v>354</v>
@@ -7080,7 +7079,7 @@
         <v>5</v>
       </c>
       <c r="K125" s="2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="L125" s="2" t="s">
         <v>354</v>
@@ -7089,10 +7088,10 @@
         <v>355</v>
       </c>
       <c r="N125" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="U125" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="126" spans="1:21" x14ac:dyDescent="0.3">
@@ -7112,7 +7111,7 @@
         <v>75</v>
       </c>
       <c r="G126" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="H126" s="2" t="s">
         <v>354</v>
@@ -7124,7 +7123,7 @@
         <v>6</v>
       </c>
       <c r="K126" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="L126" s="2" t="s">
         <v>354</v>
@@ -7133,7 +7132,7 @@
         <v>354</v>
       </c>
       <c r="N126" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="127" spans="1:21" ht="86.4" x14ac:dyDescent="0.3">
@@ -7165,7 +7164,7 @@
         <v>355</v>
       </c>
       <c r="N127" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="U127" s="2" t="s">
         <v>184</v>
@@ -7194,7 +7193,7 @@
         <v>6</v>
       </c>
       <c r="K128" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="L128" s="2" t="s">
         <v>354</v>
@@ -7203,7 +7202,7 @@
         <v>355</v>
       </c>
       <c r="N128" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="129" spans="1:21" x14ac:dyDescent="0.3">
@@ -7235,7 +7234,7 @@
         <v>355</v>
       </c>
       <c r="N129" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="130" spans="1:21" x14ac:dyDescent="0.3">
@@ -7255,7 +7254,7 @@
         <v>80</v>
       </c>
       <c r="G130" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="H130" s="2" t="s">
         <v>354</v>
@@ -7267,7 +7266,7 @@
         <v>4</v>
       </c>
       <c r="K130" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="L130" s="2" t="s">
         <v>354</v>
@@ -7276,7 +7275,7 @@
         <v>355</v>
       </c>
       <c r="N130" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="131" spans="1:21" x14ac:dyDescent="0.3">
@@ -7296,7 +7295,7 @@
         <v>81</v>
       </c>
       <c r="G131" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="H131" s="2" t="s">
         <v>354</v>
@@ -7308,7 +7307,7 @@
         <v>5</v>
       </c>
       <c r="K131" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="L131" s="2" t="s">
         <v>354</v>
@@ -7317,7 +7316,7 @@
         <v>355</v>
       </c>
       <c r="N131" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="132" spans="1:21" x14ac:dyDescent="0.3">
@@ -7337,10 +7336,10 @@
         <v>82</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="G132" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="H132" s="2" t="s">
         <v>354</v>
@@ -7352,7 +7351,7 @@
         <v>6</v>
       </c>
       <c r="K132" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="L132" s="2" t="s">
         <v>354</v>
@@ -7361,10 +7360,10 @@
         <v>355</v>
       </c>
       <c r="N132" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="P132" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="133" spans="1:21" x14ac:dyDescent="0.3">
@@ -7381,7 +7380,7 @@
         <v>105</v>
       </c>
       <c r="F133" s="10" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G133" s="10"/>
       <c r="H133" s="2" t="s">
@@ -7394,7 +7393,7 @@
         <v>6</v>
       </c>
       <c r="K133" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="L133" s="2" t="s">
         <v>354</v>
@@ -7403,7 +7402,7 @@
         <v>355</v>
       </c>
       <c r="N133" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="134" spans="1:21" x14ac:dyDescent="0.3">
@@ -7424,7 +7423,7 @@
       </c>
       <c r="F134" s="10"/>
       <c r="G134" s="10" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="H134" s="2" t="s">
         <v>354</v>
@@ -7442,7 +7441,7 @@
         <v>355</v>
       </c>
       <c r="N134" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="135" spans="1:21" x14ac:dyDescent="0.3">
@@ -7465,7 +7464,7 @@
         <v>205</v>
       </c>
       <c r="G135" s="10" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="H135" s="2" t="s">
         <v>354</v>
@@ -7477,7 +7476,7 @@
         <v>3</v>
       </c>
       <c r="K135" s="3" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="L135" s="2" t="s">
         <v>354</v>
@@ -7486,7 +7485,7 @@
         <v>355</v>
       </c>
       <c r="N135" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="136" spans="1:21" x14ac:dyDescent="0.3">
@@ -7506,7 +7505,7 @@
         <v>41</v>
       </c>
       <c r="G136" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="H136" s="2" t="s">
         <v>354</v>
@@ -7524,7 +7523,7 @@
         <v>355</v>
       </c>
       <c r="N136" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="137" spans="1:21" x14ac:dyDescent="0.3">
@@ -7550,7 +7549,7 @@
         <v>4</v>
       </c>
       <c r="K137" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="L137" s="2" t="s">
         <v>354</v>
@@ -7559,7 +7558,7 @@
         <v>355</v>
       </c>
       <c r="N137" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="138" spans="1:21" x14ac:dyDescent="0.3">
@@ -7588,10 +7587,10 @@
         <v>355</v>
       </c>
       <c r="N138" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="U138" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="139" spans="1:21" ht="72" x14ac:dyDescent="0.3">
@@ -7617,7 +7616,7 @@
         <v>7</v>
       </c>
       <c r="K139" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="L139" s="2" t="s">
         <v>354</v>
@@ -7626,10 +7625,10 @@
         <v>355</v>
       </c>
       <c r="N139" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="R139" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="140" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
@@ -7646,7 +7645,7 @@
         <v>6</v>
       </c>
       <c r="F140" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="H140" s="2" t="s">
         <v>354</v>
@@ -7658,7 +7657,7 @@
         <v>1</v>
       </c>
       <c r="K140" s="3" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="L140" s="2" t="s">
         <v>354</v>
@@ -7667,7 +7666,7 @@
         <v>354</v>
       </c>
       <c r="N140" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="141" spans="1:21" ht="86.4" x14ac:dyDescent="0.3">
@@ -7702,7 +7701,7 @@
         <v>355</v>
       </c>
       <c r="N141" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="U141" s="2" t="s">
         <v>196</v>
@@ -7719,7 +7718,7 @@
         <v>194</v>
       </c>
       <c r="E142" s="2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="H142" s="2" t="s">
         <v>354</v>
@@ -7728,7 +7727,7 @@
         <v>362</v>
       </c>
       <c r="J142" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="L142" s="2" t="s">
         <v>355</v>
@@ -7737,7 +7736,7 @@
         <v>355</v>
       </c>
       <c r="N142" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="U142" s="12" t="s">
         <v>363</v>
@@ -7745,25 +7744,25 @@
     </row>
     <row r="143" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B143" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="E143" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="E143" s="2" t="s">
+      <c r="H143" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="I143" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="H143" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="I143" s="2" t="s">
-        <v>400</v>
-      </c>
       <c r="J143" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="K143" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="L143" s="2" t="s">
         <v>354</v>
@@ -7772,97 +7771,97 @@
         <v>355</v>
       </c>
       <c r="N143" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="U143" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="144" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E144" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="H144" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="I144" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="H144" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="I144" s="2" t="s">
+      <c r="K144" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="L144" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="M144" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="N144" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="U144" s="2" t="s">
         <v>396</v>
-      </c>
-      <c r="K144" s="2" t="s">
-        <v>451</v>
-      </c>
-      <c r="L144" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="M144" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="N144" s="2" t="s">
-        <v>445</v>
-      </c>
-      <c r="U144" s="2" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="145" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E145" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H145" s="2" t="s">
         <v>354</v>
       </c>
       <c r="I145" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="K145" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="L145" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="M145" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="N145" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="U145" s="2" t="s">
         <v>396</v>
-      </c>
-      <c r="K145" s="2" t="s">
-        <v>450</v>
-      </c>
-      <c r="L145" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="M145" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="N145" s="2" t="s">
-        <v>445</v>
-      </c>
-      <c r="U145" s="2" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="146" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E146" s="2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="H146" s="2" t="s">
         <v>354</v>
       </c>
       <c r="I146" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="J146" s="2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="K146" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="L146" s="2" t="s">
         <v>354</v>
@@ -7871,33 +7870,33 @@
         <v>355</v>
       </c>
       <c r="N146" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="U146" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="147" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="E147" s="2" t="s">
         <v>458</v>
       </c>
-      <c r="B147" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="E147" s="2" t="s">
-        <v>459</v>
-      </c>
       <c r="H147" s="2" t="s">
         <v>354</v>
       </c>
       <c r="I147" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="J147" s="2" t="s">
         <v>364</v>
       </c>
       <c r="K147" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="L147" s="2" t="s">
         <v>354</v>
@@ -7906,34 +7905,34 @@
         <v>355</v>
       </c>
       <c r="N147" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="148" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B148" s="2" t="s">
         <v>83</v>
       </c>
       <c r="D148" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="E148" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="E148" s="2" t="s">
+      <c r="F148" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="H148" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="I148" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="F148" s="2" t="s">
-        <v>543</v>
-      </c>
-      <c r="H148" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="I148" s="2" t="s">
+      <c r="J148" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="J148" s="2" t="s">
-        <v>413</v>
-      </c>
       <c r="L148" s="2" t="s">
         <v>354</v>
       </c>
@@ -7941,28 +7940,28 @@
         <v>355</v>
       </c>
       <c r="N148" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="149" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="E149" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="H149" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I149" s="2" t="s">
         <v>446</v>
       </c>
-      <c r="B149" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="E149" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="H149" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="I149" s="2" t="s">
+      <c r="K149" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="K149" s="2" t="s">
-        <v>448</v>
-      </c>
       <c r="L149" s="2" t="s">
         <v>355</v>
       </c>
@@ -7970,33 +7969,33 @@
         <v>354</v>
       </c>
       <c r="N149" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="U149" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="150" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E150" s="2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="H150" s="2" t="s">
         <v>354</v>
       </c>
       <c r="I150" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="J150" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K150" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="L150" s="2" t="s">
         <v>354</v>
@@ -8005,30 +8004,30 @@
         <v>355</v>
       </c>
       <c r="N150" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="151" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E151" s="2" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="H151" s="2" t="s">
         <v>354</v>
       </c>
       <c r="I151" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="J151" s="2" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="K151" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="L151" s="2" t="s">
         <v>354</v>
@@ -8037,30 +8036,30 @@
         <v>355</v>
       </c>
       <c r="N151" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="152" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E152" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="H152" s="2" t="s">
         <v>354</v>
       </c>
       <c r="I152" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="J152" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="K152" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="L152" s="2" t="s">
         <v>354</v>
@@ -8069,30 +8068,30 @@
         <v>355</v>
       </c>
       <c r="N152" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="153" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E153" s="2" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="H153" s="2" t="s">
         <v>354</v>
       </c>
       <c r="I153" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="J153" s="2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="K153" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="L153" s="2" t="s">
         <v>354</v>
@@ -8101,30 +8100,30 @@
         <v>355</v>
       </c>
       <c r="N153" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="R153" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="154" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E154" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="H154" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="I154" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="H154" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="I154" s="2" t="s">
-        <v>404</v>
-      </c>
       <c r="K154" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="L154" s="2" t="s">
         <v>354</v>
@@ -8133,24 +8132,24 @@
         <v>355</v>
       </c>
       <c r="N154" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="155" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E155" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="H155" s="2" t="s">
         <v>354</v>
       </c>
       <c r="K155" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="L155" s="2" t="s">
         <v>354</v>
@@ -8159,12 +8158,12 @@
         <v>355</v>
       </c>
       <c r="N155" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="156" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B156" s="2" t="s">
         <v>125</v>
@@ -8176,34 +8175,34 @@
         <v>139</v>
       </c>
       <c r="F156" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="H156" s="2" t="s">
         <v>354</v>
       </c>
       <c r="I156" s="2" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="J156" s="2">
         <v>6</v>
       </c>
       <c r="K156" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="L156" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="M156" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="N156" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="R156" s="2" t="s">
         <v>603</v>
       </c>
-      <c r="L156" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="M156" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="N156" s="2" t="s">
-        <v>444</v>
-      </c>
-      <c r="R156" s="2" t="s">
+      <c r="U156" s="2" t="s">
         <v>604</v>
-      </c>
-      <c r="U156" s="2" t="s">
-        <v>605</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new treatent aanloop and uitloop, version 1
</commit_message>
<xml_diff>
--- a/src/sastadev/data/methods/TARSP_Index_Current.xlsx
+++ b/src/sastadev/data/methods/TARSP_Index_Current.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\jodijk\myprograms\python\sastacode\mysastadev\src\sastadev\data\methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91BC3983-F2BC-4346-B33D-0B4526380DFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00732F77-BEF1-4709-9797-6F635CBFC53F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1852,12 +1852,6 @@
     <t>vudivers</t>
   </si>
   <si>
-    <t>//node[@pt="ww" and not(%Tarsp_kijkVU%) and ancestor::node[@cat="top" and count(.//node[%realwordnode%]) = 1 ]]</t>
-  </si>
-  <si>
-    <t>//node[@pt="n" and %realwordnode% and @lemma!="kijk"]/ancestor::node[@cat="top" and  count(.//node[%realwordnode%])=1]</t>
-  </si>
-  <si>
     <t>//node[%Tarsp_Hwwvd%]</t>
   </si>
   <si>
@@ -1919,6 +1913,12 @@
   </si>
   <si>
     <t>//node[%BezZn%]</t>
+  </si>
+  <si>
+    <t>//node[@pt="ww" and not(%Tarsp_kijkVU%) and %thisistheonlyrealword%]</t>
+  </si>
+  <si>
+    <t>//node[@pt="n" and %realwordnode% and @lemma!="kijk" and %thisistheonlyrealword%]</t>
   </si>
 </sst>
 </file>
@@ -2340,11 +2340,11 @@
   <dimension ref="A1:V156"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="G10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="G19" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
-      <selection pane="bottomRight" activeCell="K15" sqref="K15"/>
+      <selection pane="bottomRight" activeCell="K115" sqref="K115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2429,7 +2429,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>213</v>
       </c>
@@ -2476,7 +2476,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="3" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>214</v>
       </c>
@@ -2517,7 +2517,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="4" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>215</v>
       </c>
@@ -2558,7 +2558,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="5" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>216</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="6" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>217</v>
       </c>
@@ -2710,7 +2710,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="9" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>220</v>
       </c>
@@ -2736,7 +2736,7 @@
         <v>6</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>353</v>
@@ -2821,7 +2821,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="12" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>223</v>
       </c>
@@ -2850,7 +2850,7 @@
         <v>3</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>353</v>
@@ -2885,7 +2885,7 @@
         <v>5</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="L13" s="3" t="s">
         <v>353</v>
@@ -2958,7 +2958,7 @@
         <v>4</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>353</v>
@@ -3031,7 +3031,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="18" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>229</v>
       </c>
@@ -3072,7 +3072,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="19" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>230</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v>1</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>353</v>
@@ -3110,7 +3110,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="20" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>231</v>
       </c>
@@ -3165,7 +3165,7 @@
         <v>4</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="L21" s="2" t="s">
         <v>353</v>
@@ -3212,7 +3212,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="23" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>234</v>
       </c>
@@ -3253,7 +3253,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:21" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>235</v>
       </c>
@@ -3463,7 +3463,7 @@
         <v>2</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="L29" s="2" t="s">
         <v>353</v>
@@ -3478,7 +3478,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="30" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>241</v>
       </c>
@@ -3516,7 +3516,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="31" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>242</v>
       </c>
@@ -3592,7 +3592,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="33" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>244</v>
       </c>
@@ -3633,10 +3633,10 @@
         <v>442</v>
       </c>
       <c r="R33" s="2" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>245</v>
       </c>
@@ -3671,7 +3671,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="35" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>246</v>
       </c>
@@ -3741,7 +3741,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="37" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>248</v>
       </c>
@@ -3846,7 +3846,7 @@
         <v>4</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="L39" s="3" t="s">
         <v>353</v>
@@ -3858,7 +3858,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="40" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>251</v>
       </c>
@@ -3899,7 +3899,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="41" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>252</v>
       </c>
@@ -3934,7 +3934,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="42" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>253</v>
       </c>
@@ -3975,7 +3975,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="43" spans="1:21" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>254</v>
       </c>
@@ -4019,7 +4019,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="44" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>255</v>
       </c>
@@ -4054,7 +4054,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="45" spans="1:21" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>256</v>
       </c>
@@ -4089,7 +4089,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="46" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>257</v>
       </c>
@@ -4133,7 +4133,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="47" spans="1:21" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:21" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>258</v>
       </c>
@@ -4235,7 +4235,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="50" spans="1:21" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>261</v>
       </c>
@@ -4270,7 +4270,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="51" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>262</v>
       </c>
@@ -4305,7 +4305,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="52" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>263</v>
       </c>
@@ -4331,7 +4331,7 @@
         <v>2</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="L52" s="2" t="s">
         <v>353</v>
@@ -4378,7 +4378,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="54" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>265</v>
       </c>
@@ -4521,7 +4521,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="58" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>269</v>
       </c>
@@ -4562,7 +4562,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="59" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>270</v>
       </c>
@@ -4603,7 +4603,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="60" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>271</v>
       </c>
@@ -4793,7 +4793,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="65" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>276</v>
       </c>
@@ -4834,7 +4834,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="66" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>277</v>
       </c>
@@ -4875,7 +4875,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="67" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>278</v>
       </c>
@@ -4916,7 +4916,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="68" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>279</v>
       </c>
@@ -4957,7 +4957,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="69" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>280</v>
       </c>
@@ -4998,7 +4998,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="70" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>281</v>
       </c>
@@ -5039,7 +5039,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="71" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>282</v>
       </c>
@@ -5080,7 +5080,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="72" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>283</v>
       </c>
@@ -5121,7 +5121,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="73" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>284</v>
       </c>
@@ -5165,7 +5165,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="74" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>285</v>
       </c>
@@ -5241,7 +5241,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="76" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>287</v>
       </c>
@@ -5279,7 +5279,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="77" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>288</v>
       </c>
@@ -5323,7 +5323,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="78" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>289</v>
       </c>
@@ -5367,7 +5367,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="79" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>290</v>
       </c>
@@ -5408,7 +5408,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="80" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>291</v>
       </c>
@@ -5446,7 +5446,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="81" spans="1:21" ht="144" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:21" ht="144" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>292</v>
       </c>
@@ -5481,7 +5481,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="82" spans="1:21" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>293</v>
       </c>
@@ -5545,7 +5545,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="84" spans="1:21" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:21" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>295</v>
       </c>
@@ -5682,7 +5682,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="88" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>299</v>
       </c>
@@ -5720,7 +5720,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="89" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>300</v>
       </c>
@@ -5755,7 +5755,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="90" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>301</v>
       </c>
@@ -5790,7 +5790,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="91" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>386</v>
       </c>
@@ -5854,7 +5854,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="93" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>303</v>
       </c>
@@ -5895,7 +5895,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="94" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>304</v>
       </c>
@@ -5942,7 +5942,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="95" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>305</v>
       </c>
@@ -6018,7 +6018,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="97" spans="1:21" ht="129.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:21" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>307</v>
       </c>
@@ -6050,7 +6050,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="98" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>308</v>
       </c>
@@ -6085,7 +6085,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="99" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>309</v>
       </c>
@@ -6111,7 +6111,7 @@
         <v>2</v>
       </c>
       <c r="K99" s="2" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="L99" s="2" t="s">
         <v>353</v>
@@ -6126,7 +6126,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="100" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>310</v>
       </c>
@@ -6199,7 +6199,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="102" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>312</v>
       </c>
@@ -6234,7 +6234,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="103" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>313</v>
       </c>
@@ -6272,7 +6272,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="104" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>314</v>
       </c>
@@ -6345,7 +6345,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="106" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>316</v>
       </c>
@@ -6389,7 +6389,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="107" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>317</v>
       </c>
@@ -6430,7 +6430,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="108" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>318</v>
       </c>
@@ -6497,7 +6497,7 @@
         <v>6</v>
       </c>
       <c r="K109" s="3" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="L109" s="2" t="s">
         <v>353</v>
@@ -6689,7 +6689,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="115" spans="1:21" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>325</v>
       </c>
@@ -6712,7 +6712,7 @@
         <v>1</v>
       </c>
       <c r="K115" s="3" t="s">
-        <v>588</v>
+        <v>608</v>
       </c>
       <c r="L115" s="3" t="s">
         <v>353</v>
@@ -6727,7 +6727,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="116" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>326</v>
       </c>
@@ -6821,7 +6821,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="119" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>329</v>
       </c>
@@ -6859,7 +6859,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="120" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>330</v>
       </c>
@@ -6923,7 +6923,7 @@
         <v>4</v>
       </c>
       <c r="K121" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="L121" s="2" t="s">
         <v>353</v>
@@ -6970,7 +6970,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="123" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>333</v>
       </c>
@@ -7005,7 +7005,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="124" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>334</v>
       </c>
@@ -7022,7 +7022,7 @@
         <v>71</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="G124" s="2" t="s">
         <v>570</v>
@@ -7049,7 +7049,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="125" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>335</v>
       </c>
@@ -7093,7 +7093,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="126" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>336</v>
       </c>
@@ -7236,7 +7236,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="130" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>340</v>
       </c>
@@ -7277,7 +7277,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="131" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>341</v>
       </c>
@@ -7318,7 +7318,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="132" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>342</v>
       </c>
@@ -7404,7 +7404,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="134" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>344</v>
       </c>
@@ -7443,7 +7443,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="135" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>345</v>
       </c>
@@ -7525,7 +7525,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="137" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>347</v>
       </c>
@@ -7592,7 +7592,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="139" spans="1:21" ht="72" hidden="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:21" ht="72" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>349</v>
       </c>
@@ -7630,7 +7630,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="140" spans="1:21" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>350</v>
       </c>
@@ -7656,7 +7656,7 @@
         <v>1</v>
       </c>
       <c r="K140" s="3" t="s">
-        <v>589</v>
+        <v>609</v>
       </c>
       <c r="L140" s="2" t="s">
         <v>353</v>
@@ -7741,7 +7741,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="143" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
         <v>390</v>
       </c>
@@ -7776,7 +7776,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="144" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
         <v>391</v>
       </c>
@@ -7808,7 +7808,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="145" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
         <v>392</v>
       </c>
@@ -7840,7 +7840,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="146" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
         <v>400</v>
       </c>
@@ -7875,7 +7875,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="147" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
         <v>456</v>
       </c>
@@ -7933,7 +7933,7 @@
         <v>411</v>
       </c>
       <c r="K148" s="2" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="L148" s="2" t="s">
         <v>353</v>
@@ -7977,7 +7977,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="150" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
         <v>458</v>
       </c>
@@ -8009,7 +8009,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="151" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
         <v>459</v>
       </c>
@@ -8041,7 +8041,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="152" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
         <v>460</v>
       </c>
@@ -8073,7 +8073,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="153" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
         <v>461</v>
       </c>
@@ -8108,7 +8108,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="154" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
         <v>466</v>
       </c>
@@ -8137,7 +8137,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="155" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
         <v>489</v>
       </c>
@@ -8163,9 +8163,9 @@
         <v>443</v>
       </c>
     </row>
-    <row r="156" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="B156" s="2" t="s">
         <v>125</v>
@@ -8183,37 +8183,32 @@
         <v>353</v>
       </c>
       <c r="I156" s="2" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="J156" s="2">
         <v>6</v>
       </c>
       <c r="K156" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="L156" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="M156" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="N156" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="R156" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="U156" s="2" t="s">
         <v>599</v>
-      </c>
-      <c r="L156" s="2" t="s">
-        <v>353</v>
-      </c>
-      <c r="M156" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="N156" s="2" t="s">
-        <v>442</v>
-      </c>
-      <c r="R156" s="2" t="s">
-        <v>600</v>
-      </c>
-      <c r="U156" s="2" t="s">
-        <v>601</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:V156" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="Wg"/>
-      </filters>
-    </filterColumn>
     <filterColumn colId="11">
       <filters>
         <filter val="yes"/>

</xml_diff>

<commit_message>
OvWG4 and related updates
</commit_message>
<xml_diff>
--- a/src/sastadev/data/methods/TARSP_Index_Current.xlsx
+++ b/src/sastadev/data/methods/TARSP_Index_Current.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\jodijk\myprograms\python\sastacode\mysastadev\src\sastadev\data\methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00732F77-BEF1-4709-9797-6F635CBFC53F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72B7A31-07D6-4FCB-803F-AD59B8CC93CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1609" uniqueCount="610">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1610" uniqueCount="611">
   <si>
     <t>Item</t>
   </si>
@@ -1509,9 +1509,6 @@
   </si>
   <si>
     <t>]</t>
-  </si>
-  <si>
-    <t>// node[@rel="mod" and (not(@lemma) or (@lemma!="ook" and @lemma!="dan")) and parent::node[@cat="np" and node[@rel="hd" and @pt!="ww"]] and @begin &gt;= ../node[@rel="hd"]/@end]</t>
   </si>
   <si>
     <t>mktarspform</t>
@@ -1919,6 +1916,12 @@
   </si>
   <si>
     <t>//node[@pt="n" and %realwordnode% and @lemma!="kijk" and %thisistheonlyrealword%]</t>
+  </si>
+  <si>
+    <t>// node[@rel="mod" and @cat="pp" and parent::node[@cat="np" and node[@rel="hd" and @pt!="ww"]] and @begin &gt;= ../node[@rel="hd"]/@end]</t>
+  </si>
+  <si>
+    <t>//node[%VzBepBvZn%]</t>
   </si>
 </sst>
 </file>
@@ -2340,11 +2343,11 @@
   <dimension ref="A1:V156"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="G19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F97" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
-      <selection pane="bottomRight" activeCell="K115" sqref="K115"/>
+      <selection pane="bottomRight" activeCell="K110" sqref="K110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2408,22 +2411,22 @@
         <v>441</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>551</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>552</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>553</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>554</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>158</v>
@@ -2443,13 +2446,13 @@
         <v>193</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>70</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>353</v>
@@ -2461,7 +2464,7 @@
         <v>3</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>353</v>
@@ -2555,7 +2558,7 @@
         <v>442</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
@@ -2619,7 +2622,7 @@
         <v>1</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>353</v>
@@ -2648,7 +2651,7 @@
         <v>193</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>353</v>
@@ -2660,7 +2663,7 @@
         <v>1</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>354</v>
@@ -2736,7 +2739,7 @@
         <v>6</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>353</v>
@@ -2774,7 +2777,7 @@
         <v>4</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>353</v>
@@ -2838,7 +2841,7 @@
         <v>38</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>353</v>
@@ -2850,7 +2853,7 @@
         <v>3</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>353</v>
@@ -2885,7 +2888,7 @@
         <v>5</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="L13" s="3" t="s">
         <v>353</v>
@@ -2958,7 +2961,7 @@
         <v>4</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>353</v>
@@ -2987,7 +2990,7 @@
         <v>353</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>354</v>
@@ -3086,7 +3089,7 @@
         <v>389</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>353</v>
@@ -3098,7 +3101,7 @@
         <v>1</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>353</v>
@@ -3165,7 +3168,7 @@
         <v>4</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="L21" s="2" t="s">
         <v>353</v>
@@ -3200,7 +3203,7 @@
         <v>3</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="L22" s="2" t="s">
         <v>353</v>
@@ -3229,7 +3232,7 @@
         <v>47</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>353</v>
@@ -3241,7 +3244,7 @@
         <v>5</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="L23" s="2" t="s">
         <v>353</v>
@@ -3273,7 +3276,7 @@
         <v>26</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>353</v>
@@ -3285,7 +3288,7 @@
         <v>2</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>353</v>
@@ -3297,7 +3300,7 @@
         <v>442</v>
       </c>
       <c r="U24" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="25" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
@@ -3355,7 +3358,7 @@
         <v>4</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="L26" s="3" t="s">
         <v>353</v>
@@ -3463,7 +3466,7 @@
         <v>2</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="L29" s="2" t="s">
         <v>353</v>
@@ -3501,7 +3504,7 @@
         <v>3</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="L30" s="2" t="s">
         <v>353</v>
@@ -3551,7 +3554,7 @@
         <v>442</v>
       </c>
       <c r="R31" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
@@ -3621,7 +3624,7 @@
         <v>3</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L33" s="2" t="s">
         <v>353</v>
@@ -3633,7 +3636,7 @@
         <v>442</v>
       </c>
       <c r="R33" s="2" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.3">
@@ -3659,7 +3662,7 @@
         <v>6</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="L34" s="2" t="s">
         <v>353</v>
@@ -3764,7 +3767,7 @@
         <v>3</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="L37" s="2" t="s">
         <v>353</v>
@@ -3793,7 +3796,7 @@
         <v>209</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>353</v>
@@ -3805,7 +3808,7 @@
         <v>363</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="L38" s="3" t="s">
         <v>353</v>
@@ -3834,7 +3837,7 @@
         <v>210</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>353</v>
@@ -3846,7 +3849,7 @@
         <v>4</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="L39" s="3" t="s">
         <v>353</v>
@@ -3872,7 +3875,7 @@
         <v>145</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>353</v>
@@ -3884,7 +3887,7 @@
         <v>3</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="L40" s="3" t="s">
         <v>353</v>
@@ -4004,7 +4007,7 @@
         <v>3</v>
       </c>
       <c r="K43" s="3" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="L43" s="2" t="s">
         <v>353</v>
@@ -4042,7 +4045,7 @@
         <v>3</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="L44" s="2" t="s">
         <v>353</v>
@@ -4077,7 +4080,7 @@
         <v>6</v>
       </c>
       <c r="K45" s="3" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="L45" s="2" t="s">
         <v>353</v>
@@ -4109,7 +4112,7 @@
         <v>202</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="H46" s="2" t="s">
         <v>353</v>
@@ -4121,7 +4124,7 @@
         <v>2</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="L46" s="2" t="s">
         <v>353</v>
@@ -4185,7 +4188,7 @@
         <v>354</v>
       </c>
       <c r="K48" s="3" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="L48" s="3" t="s">
         <v>354</v>
@@ -4293,7 +4296,7 @@
         <v>4</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="L51" s="2" t="s">
         <v>353</v>
@@ -4331,7 +4334,7 @@
         <v>2</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="L52" s="2" t="s">
         <v>353</v>
@@ -4366,7 +4369,7 @@
         <v>6</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>483</v>
+        <v>609</v>
       </c>
       <c r="L53" s="2" t="s">
         <v>353</v>
@@ -4404,7 +4407,7 @@
         <v>6</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="L54" s="2" t="s">
         <v>353</v>
@@ -4483,7 +4486,7 @@
         <v>442</v>
       </c>
       <c r="R56" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="57" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
@@ -4509,7 +4512,7 @@
         <v>1</v>
       </c>
       <c r="K57" s="3" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="L57" s="2" t="s">
         <v>354</v>
@@ -4538,7 +4541,7 @@
         <v>21</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="H58" s="2" t="s">
         <v>353</v>
@@ -4550,7 +4553,7 @@
         <v>2</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="L58" s="2" t="s">
         <v>353</v>
@@ -4579,7 +4582,7 @@
         <v>39</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="H59" s="2" t="s">
         <v>353</v>
@@ -4591,7 +4594,7 @@
         <v>3</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="L59" s="2" t="s">
         <v>353</v>
@@ -4641,7 +4644,7 @@
         <v>442</v>
       </c>
       <c r="R60" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="61" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
@@ -4822,7 +4825,7 @@
         <v>2</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="L65" s="2" t="s">
         <v>353</v>
@@ -4851,7 +4854,7 @@
         <v>25</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="H66" s="2" t="s">
         <v>353</v>
@@ -4863,7 +4866,7 @@
         <v>2</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="L66" s="2" t="s">
         <v>353</v>
@@ -4892,7 +4895,7 @@
         <v>35</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="H67" s="2" t="s">
         <v>353</v>
@@ -4904,7 +4907,7 @@
         <v>3</v>
       </c>
       <c r="K67" s="3" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="L67" s="2" t="s">
         <v>353</v>
@@ -4933,7 +4936,7 @@
         <v>44</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="H68" s="2" t="s">
         <v>353</v>
@@ -4974,7 +4977,7 @@
         <v>43</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="H69" s="2" t="s">
         <v>353</v>
@@ -5015,7 +5018,7 @@
         <v>32</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="H70" s="2" t="s">
         <v>353</v>
@@ -5027,7 +5030,7 @@
         <v>3</v>
       </c>
       <c r="K70" s="3" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="L70" s="2" t="s">
         <v>353</v>
@@ -5056,7 +5059,7 @@
         <v>46</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="H71" s="2" t="s">
         <v>353</v>
@@ -5068,7 +5071,7 @@
         <v>5</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="L71" s="2" t="s">
         <v>353</v>
@@ -5097,10 +5100,10 @@
         <v>405</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="H72" s="2" t="s">
         <v>353</v>
@@ -5138,10 +5141,10 @@
         <v>188</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="H73" s="2" t="s">
         <v>353</v>
@@ -5153,7 +5156,7 @@
         <v>3</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="L73" s="2" t="s">
         <v>353</v>
@@ -5203,7 +5206,7 @@
         <v>442</v>
       </c>
       <c r="R74" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.3">
@@ -5238,7 +5241,7 @@
         <v>442</v>
       </c>
       <c r="R75" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.3">
@@ -5296,10 +5299,10 @@
         <v>49</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="H77" s="2" t="s">
         <v>353</v>
@@ -5311,7 +5314,7 @@
         <v>4</v>
       </c>
       <c r="K77" s="3" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="L77" s="2" t="s">
         <v>353</v>
@@ -5340,10 +5343,10 @@
         <v>48</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="H78" s="2" t="s">
         <v>353</v>
@@ -5355,7 +5358,7 @@
         <v>5</v>
       </c>
       <c r="K78" s="3" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="L78" s="2" t="s">
         <v>353</v>
@@ -5381,7 +5384,7 @@
         <v>139</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H79" s="2" t="s">
         <v>353</v>
@@ -5405,7 +5408,7 @@
         <v>442</v>
       </c>
       <c r="R79" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="80" spans="1:21" x14ac:dyDescent="0.3">
@@ -5469,7 +5472,7 @@
         <v>4</v>
       </c>
       <c r="K81" s="3" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="L81" s="3" t="s">
         <v>353</v>
@@ -5507,7 +5510,7 @@
         <v>4</v>
       </c>
       <c r="K82" s="3" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="L82" s="2" t="s">
         <v>353</v>
@@ -5583,7 +5586,7 @@
         <v>442</v>
       </c>
       <c r="R84" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="85" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
@@ -5696,7 +5699,7 @@
         <v>381</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="H88" s="2" t="s">
         <v>353</v>
@@ -5708,7 +5711,7 @@
         <v>1</v>
       </c>
       <c r="K88" s="3" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="L88" s="2" t="s">
         <v>353</v>
@@ -5743,7 +5746,7 @@
         <v>1</v>
       </c>
       <c r="K89" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="L89" s="2" t="s">
         <v>353</v>
@@ -5804,7 +5807,7 @@
         <v>382</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="H91" s="2" t="s">
         <v>353</v>
@@ -5842,7 +5845,7 @@
         <v>353</v>
       </c>
       <c r="K92" s="2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="L92" s="2" t="s">
         <v>354</v>
@@ -5883,7 +5886,7 @@
         <v>6</v>
       </c>
       <c r="K93" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="L93" s="2" t="s">
         <v>353</v>
@@ -5912,10 +5915,10 @@
         <v>24</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="H94" s="2" t="s">
         <v>353</v>
@@ -5927,7 +5930,7 @@
         <v>2</v>
       </c>
       <c r="K94" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="L94" s="2" t="s">
         <v>353</v>
@@ -5959,7 +5962,7 @@
         <v>45</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="H95" s="2" t="s">
         <v>353</v>
@@ -5971,7 +5974,7 @@
         <v>5</v>
       </c>
       <c r="K95" s="2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L95" s="2" t="s">
         <v>353</v>
@@ -6038,7 +6041,7 @@
         <v>451</v>
       </c>
       <c r="K97" s="3" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="L97" s="3" t="s">
         <v>353</v>
@@ -6082,7 +6085,7 @@
         <v>442</v>
       </c>
       <c r="R98" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="99" spans="1:21" x14ac:dyDescent="0.3">
@@ -6111,7 +6114,7 @@
         <v>2</v>
       </c>
       <c r="K99" s="2" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="L99" s="2" t="s">
         <v>353</v>
@@ -6187,7 +6190,7 @@
         <v>5</v>
       </c>
       <c r="K101" s="3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="L101" s="2" t="s">
         <v>353</v>
@@ -6222,7 +6225,7 @@
         <v>4</v>
       </c>
       <c r="K102" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="L102" s="2" t="s">
         <v>353</v>
@@ -6310,7 +6313,7 @@
         <v>454</v>
       </c>
       <c r="R104" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="U104" s="2" t="s">
         <v>167</v>
@@ -6374,7 +6377,7 @@
         <v>4</v>
       </c>
       <c r="K106" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="L106" s="2" t="s">
         <v>353</v>
@@ -6415,7 +6418,7 @@
         <v>5</v>
       </c>
       <c r="K107" s="3" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="L107" s="2" t="s">
         <v>353</v>
@@ -6456,7 +6459,7 @@
         <v>6</v>
       </c>
       <c r="K108" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="L108" s="2" t="s">
         <v>353</v>
@@ -6497,7 +6500,7 @@
         <v>6</v>
       </c>
       <c r="K109" s="3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="L109" s="2" t="s">
         <v>353</v>
@@ -6531,7 +6534,9 @@
       <c r="J110" s="2">
         <v>7</v>
       </c>
-      <c r="K110" s="9"/>
+      <c r="K110" s="9" t="s">
+        <v>610</v>
+      </c>
       <c r="L110" s="10" t="s">
         <v>353</v>
       </c>
@@ -6542,7 +6547,7 @@
         <v>442</v>
       </c>
       <c r="R110" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="111" spans="1:21" x14ac:dyDescent="0.3">
@@ -6568,7 +6573,7 @@
         <v>4</v>
       </c>
       <c r="K111" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="L111" s="2" t="s">
         <v>353</v>
@@ -6604,7 +6609,7 @@
         <v>3</v>
       </c>
       <c r="K112" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="L112" s="2" t="s">
         <v>353</v>
@@ -6616,7 +6621,7 @@
         <v>442</v>
       </c>
       <c r="U112" s="3" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="113" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
@@ -6665,7 +6670,7 @@
         <v>193</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="H114" s="2" t="s">
         <v>353</v>
@@ -6677,7 +6682,7 @@
         <v>1</v>
       </c>
       <c r="K114" s="3" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="L114" s="2" t="s">
         <v>354</v>
@@ -6712,7 +6717,7 @@
         <v>1</v>
       </c>
       <c r="K115" s="3" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="L115" s="3" t="s">
         <v>353</v>
@@ -6744,7 +6749,7 @@
         <v>79</v>
       </c>
       <c r="G116" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="H116" s="2" t="s">
         <v>353</v>
@@ -6876,7 +6881,7 @@
         <v>40</v>
       </c>
       <c r="G120" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H120" s="2" t="s">
         <v>353</v>
@@ -6888,7 +6893,7 @@
         <v>3</v>
       </c>
       <c r="K120" s="3" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="L120" s="2" t="s">
         <v>353</v>
@@ -6923,7 +6928,7 @@
         <v>4</v>
       </c>
       <c r="K121" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="L121" s="2" t="s">
         <v>353</v>
@@ -6958,7 +6963,7 @@
         <v>3</v>
       </c>
       <c r="K122" s="2" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="L122" s="2" t="s">
         <v>354</v>
@@ -7022,10 +7027,10 @@
         <v>71</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="G124" s="2" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H124" s="2" t="s">
         <v>353</v>
@@ -7037,7 +7042,7 @@
         <v>4</v>
       </c>
       <c r="K124" s="3" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="L124" s="2" t="s">
         <v>353</v>
@@ -7066,7 +7071,7 @@
         <v>73</v>
       </c>
       <c r="G125" s="2" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H125" s="2" t="s">
         <v>353</v>
@@ -7078,7 +7083,7 @@
         <v>5</v>
       </c>
       <c r="K125" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L125" s="2" t="s">
         <v>353</v>
@@ -7110,7 +7115,7 @@
         <v>75</v>
       </c>
       <c r="G126" s="2" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H126" s="2" t="s">
         <v>353</v>
@@ -7122,7 +7127,7 @@
         <v>6</v>
       </c>
       <c r="K126" s="2" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="L126" s="2" t="s">
         <v>353</v>
@@ -7192,7 +7197,7 @@
         <v>6</v>
       </c>
       <c r="K128" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="L128" s="2" t="s">
         <v>353</v>
@@ -7253,7 +7258,7 @@
         <v>80</v>
       </c>
       <c r="G130" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="H130" s="2" t="s">
         <v>353</v>
@@ -7265,7 +7270,7 @@
         <v>4</v>
       </c>
       <c r="K130" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="L130" s="2" t="s">
         <v>353</v>
@@ -7294,7 +7299,7 @@
         <v>81</v>
       </c>
       <c r="G131" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="H131" s="2" t="s">
         <v>353</v>
@@ -7306,7 +7311,7 @@
         <v>5</v>
       </c>
       <c r="K131" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="L131" s="2" t="s">
         <v>353</v>
@@ -7338,7 +7343,7 @@
         <v>440</v>
       </c>
       <c r="G132" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="H132" s="2" t="s">
         <v>353</v>
@@ -7350,7 +7355,7 @@
         <v>6</v>
       </c>
       <c r="K132" s="2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="L132" s="2" t="s">
         <v>353</v>
@@ -7422,7 +7427,7 @@
       </c>
       <c r="F134" s="10"/>
       <c r="G134" s="10" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="H134" s="2" t="s">
         <v>353</v>
@@ -7463,7 +7468,7 @@
         <v>204</v>
       </c>
       <c r="G135" s="10" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="H135" s="2" t="s">
         <v>353</v>
@@ -7475,7 +7480,7 @@
         <v>3</v>
       </c>
       <c r="K135" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="L135" s="2" t="s">
         <v>353</v>
@@ -7504,7 +7509,7 @@
         <v>41</v>
       </c>
       <c r="G136" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="H136" s="2" t="s">
         <v>353</v>
@@ -7627,7 +7632,7 @@
         <v>442</v>
       </c>
       <c r="R139" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="140" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
@@ -7644,7 +7649,7 @@
         <v>6</v>
       </c>
       <c r="F140" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="H140" s="2" t="s">
         <v>353</v>
@@ -7656,7 +7661,7 @@
         <v>1</v>
       </c>
       <c r="K140" s="3" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="L140" s="2" t="s">
         <v>353</v>
@@ -7717,7 +7722,7 @@
         <v>194</v>
       </c>
       <c r="E142" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="H142" s="2" t="s">
         <v>353</v>
@@ -7921,7 +7926,7 @@
         <v>409</v>
       </c>
       <c r="F148" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H148" s="2" t="s">
         <v>353</v>
@@ -7933,7 +7938,7 @@
         <v>411</v>
       </c>
       <c r="K148" s="2" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="L148" s="2" t="s">
         <v>353</v>
@@ -8105,7 +8110,7 @@
         <v>443</v>
       </c>
       <c r="R153" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="154" spans="1:21" x14ac:dyDescent="0.3">
@@ -8139,19 +8144,19 @@
     </row>
     <row r="155" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E155" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="H155" s="2" t="s">
         <v>353</v>
       </c>
       <c r="K155" s="2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="L155" s="2" t="s">
         <v>353</v>
@@ -8165,7 +8170,7 @@
     </row>
     <row r="156" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B156" s="2" t="s">
         <v>125</v>
@@ -8177,34 +8182,34 @@
         <v>139</v>
       </c>
       <c r="F156" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H156" s="2" t="s">
         <v>353</v>
       </c>
       <c r="I156" s="2" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="J156" s="2">
         <v>6</v>
       </c>
       <c r="K156" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="L156" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="M156" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="N156" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="R156" s="2" t="s">
         <v>597</v>
       </c>
-      <c r="L156" s="2" t="s">
-        <v>353</v>
-      </c>
-      <c r="M156" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="N156" s="2" t="s">
-        <v>442</v>
-      </c>
-      <c r="R156" s="2" t="s">
+      <c r="U156" s="2" t="s">
         <v>598</v>
-      </c>
-      <c r="U156" s="2" t="s">
-        <v>599</v>
       </c>
     </row>
   </sheetData>

</xml_diff>